<commit_message>
Added a logos directory
</commit_message>
<xml_diff>
--- a/documentation/Documentation.xlsx
+++ b/documentation/Documentation.xlsx
@@ -8,16 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Ratliff Drive/Projects/excella-badges/documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEFB2694-7470-7541-B0D4-9ED839A01D61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1C4CDC4-3370-C44A-957B-E0C576E7BD7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38400" yWindow="-3600" windowWidth="38400" windowHeight="21600" xr2:uid="{8A12091D-5711-3445-86BD-2D461F98DB31}"/>
   </bookViews>
   <sheets>
     <sheet name="ERD Diagram" sheetId="1" r:id="rId1"/>
     <sheet name="API" sheetId="3" r:id="rId2"/>
-    <sheet name="Models" sheetId="4" r:id="rId3"/>
-    <sheet name="Seed Data" sheetId="5" r:id="rId4"/>
+    <sheet name="User" sheetId="5" r:id="rId3"/>
+    <sheet name="Badge" sheetId="6" r:id="rId4"/>
+    <sheet name="Achievement" sheetId="7" r:id="rId5"/>
+    <sheet name="Requirement" sheetId="8" r:id="rId6"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">API!$A$41:$E$49</definedName>
+  </definedNames>
   <calcPr calcId="181029"/>
   <fileRecoveryPr repairLoad="1"/>
   <extLst>
@@ -39,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="131">
   <si>
     <t>Excella Badges</t>
   </si>
@@ -71,21 +76,12 @@
     <t>Python</t>
   </si>
   <si>
-    <t>Achievement</t>
-  </si>
-  <si>
     <t>Certification</t>
   </si>
   <si>
     <t>Capability</t>
   </si>
   <si>
-    <t>SkillLevel</t>
-  </si>
-  <si>
-    <t>Last Updated 03/08/22</t>
-  </si>
-  <si>
     <t>API Schema v1.0</t>
   </si>
   <si>
@@ -107,54 +103,6 @@
     <t>User[]</t>
   </si>
   <si>
-    <t>id</t>
-  </si>
-  <si>
-    <t>first_name</t>
-  </si>
-  <si>
-    <t>string</t>
-  </si>
-  <si>
-    <t>number</t>
-  </si>
-  <si>
-    <t>first name of the user</t>
-  </si>
-  <si>
-    <t>primary key</t>
-  </si>
-  <si>
-    <t>last_name</t>
-  </si>
-  <si>
-    <t>email</t>
-  </si>
-  <si>
-    <t>title</t>
-  </si>
-  <si>
-    <t>role</t>
-  </si>
-  <si>
-    <t>consultant, senior, lead, etc..</t>
-  </si>
-  <si>
-    <t>developer, agilist, capability lead</t>
-  </si>
-  <si>
-    <t>java, .net, python, agile, marketing</t>
-  </si>
-  <si>
-    <t>primary_skill</t>
-  </si>
-  <si>
-    <t>excella email address</t>
-  </si>
-  <si>
-    <t>last name of user</t>
-  </si>
-  <si>
     <t>Return list of all users</t>
   </si>
   <si>
@@ -224,123 +172,15 @@
     <t>Returns list of badges for a given skill</t>
   </si>
   <si>
-    <t>/userbadge</t>
-  </si>
-  <si>
-    <t>UserBadge[]</t>
-  </si>
-  <si>
-    <t>Returns list of all userbadges</t>
-  </si>
-  <si>
-    <t>Returns list of userbadges for a given user</t>
-  </si>
-  <si>
-    <t>/userbadge/user/{user_id}</t>
-  </si>
-  <si>
-    <t>/userbadge/user/{user_id}/capability/{capability_id}</t>
-  </si>
-  <si>
-    <t>Returns list of userbadges for a given user and capability</t>
-  </si>
-  <si>
-    <t>/userbadge/user/{user_id}/skill/{skill_id}</t>
-  </si>
-  <si>
-    <t>Returns list of userbadges for a given user and skill</t>
-  </si>
-  <si>
-    <t>/userbadge/{id}</t>
-  </si>
-  <si>
-    <t>UserBadge</t>
-  </si>
-  <si>
-    <t>Returns a userbadge given the id</t>
-  </si>
-  <si>
-    <t>POST</t>
-  </si>
-  <si>
     <t>/authenticate</t>
   </si>
   <si>
-    <t>{ "email": string, "password": string }</t>
-  </si>
-  <si>
     <t>Uses passport saml auth</t>
   </si>
   <si>
     <t>Token</t>
   </si>
   <si>
-    <t>name</t>
-  </si>
-  <si>
-    <t>icon</t>
-  </si>
-  <si>
-    <t>image</t>
-  </si>
-  <si>
-    <t>capability_id</t>
-  </si>
-  <si>
-    <t>fk to capability</t>
-  </si>
-  <si>
-    <t>badge_type_id</t>
-  </si>
-  <si>
-    <t>fk to badge type</t>
-  </si>
-  <si>
-    <t>skill_level_id</t>
-  </si>
-  <si>
-    <t>fk to skill level</t>
-  </si>
-  <si>
-    <t>notes</t>
-  </si>
-  <si>
-    <t>archived</t>
-  </si>
-  <si>
-    <t>boolean</t>
-  </si>
-  <si>
-    <t>pk</t>
-  </si>
-  <si>
-    <t>name of skill level</t>
-  </si>
-  <si>
-    <t>name of the capability</t>
-  </si>
-  <si>
-    <t>BadgeType</t>
-  </si>
-  <si>
-    <t>type of badge</t>
-  </si>
-  <si>
-    <t>user_id</t>
-  </si>
-  <si>
-    <t>fk to User</t>
-  </si>
-  <si>
-    <t>badge_id</t>
-  </si>
-  <si>
-    <t>fk to Badge</t>
-  </si>
-  <si>
-    <t>additional notes about achievement</t>
-  </si>
-  <si>
     <t>Challege</t>
   </si>
   <si>
@@ -368,9 +208,6 @@
     <t>Kanban</t>
   </si>
   <si>
-    <t>name of the discipline</t>
-  </si>
-  <si>
     <t>/discipline</t>
   </si>
   <si>
@@ -392,80 +229,221 @@
     <t>/badge/discipline/{id}</t>
   </si>
   <si>
-    <t>Solutions Architect</t>
-  </si>
-  <si>
-    <t>DevOps</t>
-  </si>
-  <si>
-    <t>Design</t>
-  </si>
-  <si>
-    <t>Ruby</t>
-  </si>
-  <si>
-    <t>Angular</t>
-  </si>
-  <si>
-    <t>React</t>
-  </si>
-  <si>
-    <t>Vue</t>
-  </si>
-  <si>
-    <t>Jquery</t>
-  </si>
-  <si>
-    <t>Java Spring</t>
-  </si>
-  <si>
-    <t>JavaScript</t>
-  </si>
-  <si>
-    <t>Django</t>
-  </si>
-  <si>
-    <t>Scrum</t>
-  </si>
-  <si>
-    <t>AWS</t>
-  </si>
-  <si>
-    <t>Jenkins</t>
-  </si>
-  <si>
-    <t>SSO</t>
-  </si>
-  <si>
-    <t>Azure</t>
-  </si>
-  <si>
-    <t>Heroku</t>
-  </si>
-  <si>
-    <t>Data Engineering</t>
-  </si>
-  <si>
-    <t>Capability Lead</t>
-  </si>
-  <si>
-    <t>Interviewing</t>
-  </si>
-  <si>
-    <t>System Design</t>
-  </si>
-  <si>
-    <t>Xpert</t>
-  </si>
-  <si>
     <t>Last Updated 03/11/22</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Returns list of all requirements for a given badge</t>
+  </si>
+  <si>
+    <t>Checklist[]</t>
+  </si>
+  <si>
+    <t>Requirements[]</t>
+  </si>
+  <si>
+    <t>Requirement</t>
+  </si>
+  <si>
+    <t>Returns a single requirement given a requirement id</t>
+  </si>
+  <si>
+    <t>/requirement/badge/{badgeid}</t>
+  </si>
+  <si>
+    <t>/requirement/{id}</t>
+  </si>
+  <si>
+    <t>/checklist/user/{userid}/badge/{badgeid}</t>
+  </si>
+  <si>
+    <t>/checklist/{id}</t>
+  </si>
+  <si>
+    <t>Checklist</t>
+  </si>
+  <si>
+    <t>Returns a single checklist requirement</t>
+  </si>
+  <si>
+    <t>Public/Private</t>
+  </si>
+  <si>
+    <t>Public</t>
+  </si>
+  <si>
+    <t>Put</t>
+  </si>
+  <si>
+    <t>Result</t>
+  </si>
+  <si>
+    <t>Updates an existing badge</t>
+  </si>
+  <si>
+    <t>Private</t>
+  </si>
+  <si>
+    <t>Post</t>
+  </si>
+  <si>
+    <t>Creates a new badge</t>
+  </si>
+  <si>
+    <t>Badge Routes</t>
+  </si>
+  <si>
+    <t>Disclipine Routes</t>
+  </si>
+  <si>
+    <t>Capability Routes</t>
+  </si>
+  <si>
+    <t>Skilllevel Routes</t>
+  </si>
+  <si>
+    <t>User Routes</t>
+  </si>
+  <si>
+    <t>CurrentUser Routes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     { badge: Badge }</t>
+  </si>
+  <si>
+    <t>Requirement Routes</t>
+  </si>
+  <si>
+    <t>Delete</t>
+  </si>
+  <si>
+    <t>Checklist Routes</t>
+  </si>
+  <si>
+    <t>Returns the result of updating a badge checklist item</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     { checklist: Checklist}</t>
+  </si>
+  <si>
+    <t>/checklist</t>
+  </si>
+  <si>
+    <t>Returns a new badge checklist item</t>
+  </si>
+  <si>
+    <t>/requirement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     { requirement: Requirement}</t>
+  </si>
+  <si>
+    <t>Returns a new badge requirement item</t>
+  </si>
+  <si>
+    <t>Result from updating a requirement</t>
+  </si>
+  <si>
+    <t>Updates an existing user</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     { user: User  }</t>
+  </si>
+  <si>
+    <t>Creates a new user</t>
+  </si>
+  <si>
+    <t>/discipline/{id}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     { discipline: Discipline }</t>
+  </si>
+  <si>
+    <t>Updates an existing discipline</t>
+  </si>
+  <si>
+    <t>Creates a new discipline</t>
+  </si>
+  <si>
+    <t>Deletes a requirement</t>
+  </si>
+  <si>
+    <t>Authentication Routes</t>
+  </si>
+  <si>
+    <t>/authenciate/getToken</t>
+  </si>
+  <si>
+    <t>Returns the token of the currently authentication user</t>
+  </si>
+  <si>
+    <t>Returns list of all checklists  for a given user and badge</t>
+  </si>
+  <si>
+    <t>Returns the result of updating a requirement item</t>
+  </si>
+  <si>
+    <t>{ "email": string, "password": encrypted string }</t>
+  </si>
+  <si>
+    <t>/user/discipline/{id}</t>
+  </si>
+  <si>
+    <t>Returns list of all users that have at least one achievement in this discipline</t>
+  </si>
+  <si>
+    <t>/user/capability/{id}</t>
+  </si>
+  <si>
+    <t>Returns list of all users that have at least one achievement in a capability</t>
+  </si>
+  <si>
+    <t>achievement[]</t>
+  </si>
+  <si>
+    <t>/achievement/{id}</t>
+  </si>
+  <si>
+    <t>Returns a achievement  given the id</t>
+  </si>
+  <si>
+    <t>/achievement/user/{user_id}</t>
+  </si>
+  <si>
+    <t>Returns list of achievement  for a given user</t>
+  </si>
+  <si>
+    <t>/achievement</t>
+  </si>
+  <si>
+    <t>achievement</t>
+  </si>
+  <si>
+    <t>Returns the new achievement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      { achievement: achievement }</t>
+  </si>
+  <si>
+    <t>Updates an existing achievement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     { achievement: achievement }</t>
+  </si>
+  <si>
+    <t>Deletes an achievement</t>
+  </si>
+  <si>
+    <t>Achievement Routes</t>
+  </si>
+  <si>
+    <t>Returns list of all achievements</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -503,6 +481,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -524,12 +510,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1544,7 +1531,7 @@
           <a:pPr algn="l"/>
           <a:r>
             <a:rPr lang="en-US" sz="1000"/>
-            <a:t>UserBadges</a:t>
+            <a:t>Achievement</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -1649,7 +1636,7 @@
           <a:pPr algn="l"/>
           <a:r>
             <a:rPr lang="en-US" sz="1000"/>
-            <a:t>UserBadgeChecklist</a:t>
+            <a:t>AchievementChecklist</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -1670,7 +1657,7 @@
           <a:pPr algn="l"/>
           <a:r>
             <a:rPr lang="en-US" sz="1000"/>
-            <a:t>user_badge_id</a:t>
+            <a:t>achievement_id</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -1871,7 +1858,7 @@
           <a:pPr algn="l"/>
           <a:r>
             <a:rPr lang="en-US" sz="1000"/>
-            <a:t>BadgeRequirements</a:t>
+            <a:t>BadgeRequirement</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -2282,7 +2269,7 @@
   <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="182" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2292,7 +2279,7 @@
         <v>0</v>
       </c>
       <c r="G1" t="s">
-        <v>139</v>
+        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
@@ -2307,17 +2294,12 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="H6" s="3" t="s">
-        <v>11</v>
+        <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="H7" s="3" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="H8" s="3" t="s">
-        <v>101</v>
+        <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
@@ -2332,12 +2314,12 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="I12" s="3" t="s">
-        <v>102</v>
+        <v>47</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="I13" s="3" t="s">
-        <v>103</v>
+        <v>48</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
@@ -2347,7 +2329,7 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="I16" s="3" t="s">
-        <v>107</v>
+        <v>52</v>
       </c>
     </row>
     <row r="17" spans="9:9" x14ac:dyDescent="0.2">
@@ -2362,12 +2344,12 @@
     </row>
     <row r="19" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I19" s="3" t="s">
-        <v>108</v>
+        <v>53</v>
       </c>
     </row>
     <row r="22" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I22" s="3" t="s">
-        <v>105</v>
+        <v>50</v>
       </c>
     </row>
     <row r="23" spans="9:9" x14ac:dyDescent="0.2">
@@ -2377,7 +2359,7 @@
     </row>
     <row r="24" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I24" s="3" t="s">
-        <v>106</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -2389,749 +2371,927 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9932216B-7A50-3D46-B5D7-19265EC37A39}">
-  <dimension ref="A1:D32"/>
+  <dimension ref="A1:F71"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView topLeftCell="A40" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="E51" sqref="E51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="36.83203125" customWidth="1"/>
-    <col min="2" max="2" width="6.1640625" customWidth="1"/>
-    <col min="3" max="3" width="9.83203125" customWidth="1"/>
-    <col min="4" max="4" width="37.83203125" customWidth="1"/>
+    <col min="1" max="1" width="31" customWidth="1"/>
+    <col min="2" max="2" width="14" customWidth="1"/>
+    <col min="3" max="4" width="11.33203125" customWidth="1"/>
+    <col min="5" max="5" width="37.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="E1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B3" s="4" t="s">
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="4"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+    </row>
+    <row r="5" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="D6" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+    </row>
+    <row r="8" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E9" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="B5" s="3" t="s">
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="B10" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="B7" s="3" t="s">
+      <c r="E10" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8" s="3" t="s">
+      <c r="B11" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="D12" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D8" s="3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="3"/>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E12" s="3" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E14" s="3"/>
+    </row>
+    <row r="15" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
-        <v>112</v>
+        <v>25</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>20</v>
+        <v>78</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>113</v>
+        <v>17</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+        <v>27</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="3" t="s">
+      <c r="E17" s="3"/>
+    </row>
+    <row r="18" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" s="3"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+    </row>
+    <row r="22" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="A22" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="B18" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D19" s="3" t="s">
+      <c r="B24" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" s="3" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" s="3"/>
-      <c r="B23" s="3"/>
-      <c r="C23" s="3"/>
-      <c r="D23" s="3"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A27" s="3" t="s">
-        <v>66</v>
-      </c>
       <c r="B27" s="3" t="s">
-        <v>20</v>
+        <v>78</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>62</v>
+        <v>79</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A28" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="D28" s="3" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+        <v>49</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="B28" s="3"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="3"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A30" s="3" t="s">
+      <c r="E29" s="3"/>
+    </row>
+    <row r="30" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="A30" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="B30" s="3"/>
+      <c r="C30" s="3"/>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B31" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="B30" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="C30" s="3" t="s">
+      <c r="C31" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A33" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A34" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A35" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A36" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="E36" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="D30" s="3" t="s">
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A37" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="B37" s="3"/>
+      <c r="C37" s="3"/>
+      <c r="D37" s="3"/>
+      <c r="E37" s="3"/>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A38" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E38" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A39" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="B39" s="3"/>
+      <c r="C39" s="3"/>
+      <c r="D39" s="3"/>
+      <c r="E39" s="3"/>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A40" s="3"/>
+      <c r="B40" s="3"/>
+      <c r="C40" s="3"/>
+      <c r="D40" s="3"/>
+      <c r="E40" s="3"/>
+    </row>
+    <row r="41" spans="1:6" ht="19" x14ac:dyDescent="0.25">
+      <c r="A41" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="B41" s="3"/>
+      <c r="C41" s="3"/>
+      <c r="D41" s="3"/>
+      <c r="E41" s="3"/>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A42" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="E42" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A43" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E43" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A44" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="D44" s="3" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A31" s="3" t="s">
+      <c r="E44" s="3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A45" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B45" s="3"/>
+      <c r="C45" s="3"/>
+      <c r="D45" s="3"/>
+      <c r="E45" s="3"/>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A46" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="D46" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E46" s="3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A47" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A48" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C48" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="B31" s="3"/>
-      <c r="C31" s="3"/>
-      <c r="D31" s="3"/>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A32" s="3"/>
-      <c r="B32" s="3"/>
-      <c r="C32" s="3"/>
-      <c r="D32" s="3"/>
+      <c r="D48" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="E48" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="F48" s="3"/>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A49" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="D49" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="E49" s="3" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A50" s="3"/>
+      <c r="B50" s="3"/>
+      <c r="C50" s="3"/>
+      <c r="D50" s="3"/>
+      <c r="E50" s="3"/>
+    </row>
+    <row r="51" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="A51" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="B51" s="3"/>
+      <c r="C51" s="3"/>
+      <c r="D51" s="3"/>
+      <c r="E51" s="3"/>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A52" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D52" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="E52" s="3" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A53" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D53" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="E53" s="3" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A54" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D54" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="E54" s="3" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A55" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="B55" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C55" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="D55" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="E55" s="3" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A56" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="B56" s="3"/>
+      <c r="C56" s="3"/>
+      <c r="D56" s="3"/>
+      <c r="E56" s="3"/>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A57" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="B57" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C57" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="D57" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="E57" s="3" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A58" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="B58" s="3"/>
+      <c r="C58" s="3"/>
+      <c r="D58" s="3"/>
+      <c r="E58" s="3"/>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A59" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="B59" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C59" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="D59" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="E59" s="3" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A60" s="3"/>
+      <c r="B60" s="3"/>
+      <c r="C60" s="3"/>
+      <c r="D60" s="3"/>
+      <c r="E60" s="3"/>
+    </row>
+    <row r="61" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="A61" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="B61" s="3"/>
+      <c r="C61" s="3"/>
+      <c r="D61" s="3"/>
+      <c r="E61" s="3"/>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A62" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B62" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C62" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D62" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="E62" s="3" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A63" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B63" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C63" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D63" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="E63" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A64" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B64" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C64" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="D64" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="E64" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A65" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="B65" s="3"/>
+      <c r="C65" s="3"/>
+      <c r="D65" s="3"/>
+      <c r="E65" s="3"/>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A66" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B66" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C66" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="D66" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="E66" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="A68" s="5" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A69" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B69" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C69" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="D69" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E69" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A70" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="B70" s="3"/>
+      <c r="C70" s="3"/>
+      <c r="D70" s="3"/>
+      <c r="E70" s="3"/>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A71" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="B71" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C71" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D71" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E71" s="3" t="s">
+        <v>109</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <pageSetup orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91EEAA94-EA24-CE4C-9C6A-74D7F09A4391}">
-  <dimension ref="A1:C42"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D7FB9C0-6D9B-EA43-86CE-62488FCDBEBD}">
+  <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="16.83203125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="10.83203125" style="3"/>
-    <col min="3" max="3" width="32.1640625" style="3" customWidth="1"/>
-    <col min="4" max="16384" width="10.83203125" style="3"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" s="4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A21" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A22" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A23" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A25" s="4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A26" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A27" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A29" s="4" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A30" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B30" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C30" s="3" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A31" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="B31" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A32" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="B32" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C32" s="3" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A34" s="4" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A35" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B35" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C35" s="3" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A36" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="B36" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C36" s="3" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A38" s="4" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A39" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B39" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C39" s="3" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A40" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="B40" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C40" s="3" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A41" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="B41" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C41" s="3" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A42" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="B42" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C42" s="3" t="s">
-        <v>99</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D7FB9C0-6D9B-EA43-86CE-62488FCDBEBD}">
-  <dimension ref="A1:B51"/>
-  <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D48" sqref="D48"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
@@ -3141,233 +3301,205 @@
     <col min="3" max="16384" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="4"/>
+    </row>
+    <row r="2" spans="1:5" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+    </row>
+    <row r="3" spans="1:5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+        <v>22</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A4" s="3"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+    </row>
+    <row r="5" spans="1:5" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+    </row>
+    <row r="6" spans="1:5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A8" s="4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A10" s="3" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+        <v>36</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A10" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+        <v>113</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A13" s="3" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A14" s="3" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A15" s="3" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A16" s="3" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" s="3" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" s="4" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21" s="3" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B22" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B23" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B24" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B25" s="3" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B26" s="3" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B27" s="3" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B28" s="3" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B29" s="3" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B30" s="3" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B31" s="3" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B32" s="3" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A33" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B34" s="3" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B35" s="3" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A37" s="3" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B38" s="3" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B39" s="3" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B40" s="3" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B41" s="3" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B42" s="3" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A43" s="3" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B44" s="3" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B45" s="3" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B46" s="3" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A47" s="3" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B48" s="3" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A49" s="3" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B50" s="3" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A51" s="3" t="s">
-        <v>138</v>
-      </c>
+        <v>115</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{136FA600-DCF7-6449-AA10-6D4391292D97}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C39AF7CB-0904-5742-AE3B-3734F670F078}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H40" sqref="H40"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{548BACAB-22C5-C345-9867-53CF1A6F23C5}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I34" sqref="I34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added placeholder for controllers
</commit_message>
<xml_diff>
--- a/documentation/Documentation.xlsx
+++ b/documentation/Documentation.xlsx
@@ -8,26 +8,26 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Ratliff Drive/Projects/excella-badges/documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5309B24F-AFA9-9644-8524-4C1CCA1EFE35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D776933-4A63-4F4F-A3D4-3ABB0DA35588}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{8A12091D-5711-3445-86BD-2D461F98DB31}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" firstSheet="2" activeTab="2" xr2:uid="{8A12091D-5711-3445-86BD-2D461F98DB31}"/>
   </bookViews>
   <sheets>
     <sheet name="ERD Diagram" sheetId="1" r:id="rId1"/>
     <sheet name="Architecture" sheetId="17" r:id="rId2"/>
     <sheet name="API" sheetId="3" r:id="rId3"/>
-    <sheet name="Skilllevel" sheetId="16" r:id="rId4"/>
-    <sheet name="Capability" sheetId="15" r:id="rId5"/>
-    <sheet name="Discipline" sheetId="14" r:id="rId6"/>
-    <sheet name="Authentication" sheetId="13" r:id="rId7"/>
-    <sheet name="BadgeRequirement" sheetId="10" r:id="rId8"/>
-    <sheet name="AchievementChecklist" sheetId="12" r:id="rId9"/>
-    <sheet name="Achievement" sheetId="11" r:id="rId10"/>
-    <sheet name="User" sheetId="5" r:id="rId11"/>
+    <sheet name="User" sheetId="5" r:id="rId4"/>
+    <sheet name="Skilllevel" sheetId="16" r:id="rId5"/>
+    <sheet name="Capability" sheetId="15" r:id="rId6"/>
+    <sheet name="Discipline" sheetId="14" r:id="rId7"/>
+    <sheet name="Authentication" sheetId="13" r:id="rId8"/>
+    <sheet name="BadgeRequirement" sheetId="10" r:id="rId9"/>
+    <sheet name="AchievementChecklist" sheetId="12" r:id="rId10"/>
+    <sheet name="Achievement" sheetId="11" r:id="rId11"/>
     <sheet name="Badge" sheetId="9" r:id="rId12"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">API!$A$41:$E$49</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">API!$A$44:$E$52</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <fileRecoveryPr repairLoad="1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="483" uniqueCount="179">
   <si>
     <t>Excella Badges</t>
   </si>
@@ -566,6 +566,27 @@
   </si>
   <si>
     <t xml:space="preserve">        Service</t>
+  </si>
+  <si>
+    <t>Autenticates a user</t>
+  </si>
+  <si>
+    <t>/user/logout</t>
+  </si>
+  <si>
+    <t>/user/login</t>
+  </si>
+  <si>
+    <t>Logs a user out of the system</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     { "email": string, "password": encrypted string }</t>
+  </si>
+  <si>
+    <t>/user/email/{email}</t>
+  </si>
+  <si>
+    <t>Returns a user given an email address</t>
   </si>
 </sst>
 </file>
@@ -664,12 +685,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -684,7 +711,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -697,6 +724,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3150,10 +3178,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B4E711D-A889-F840-B38C-48F66B50F2D4}">
-  <dimension ref="A1:I26"/>
+  <dimension ref="A1:I25"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView showGridLines="0" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3253,18 +3281,18 @@
         <v>56</v>
       </c>
     </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I23" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="I24" s="3" t="s">
-        <v>53</v>
+        <v>7</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="I25" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="I26" s="3" t="s">
         <v>54</v>
       </c>
     </row>
@@ -3276,6 +3304,115 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88D14B79-96F7-D04D-9879-B8E70751AAF2}">
+  <dimension ref="A2:E9"/>
+  <sheetViews>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="31.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{121AAD50-1F3E-354D-A82B-FE61577E596D}">
   <dimension ref="A2:F12"/>
   <sheetViews>
@@ -3433,189 +3570,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D7FB9C0-6D9B-EA43-86CE-62488FCDBEBD}">
-  <dimension ref="A2:E21"/>
-  <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="16.33203125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="18" style="3" customWidth="1"/>
-    <col min="3" max="16384" width="10.83203125" style="3"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="4"/>
-    </row>
-    <row r="4" spans="1:5" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-    </row>
-    <row r="5" spans="1:5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-    </row>
-    <row r="7" spans="1:5" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-    </row>
-    <row r="8" spans="1:5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A8" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A9" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A10" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A11" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A12" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A21" s="4"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -3839,10 +3793,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9932216B-7A50-3D46-B5D7-19265EC37A39}">
-  <dimension ref="A1:F74"/>
+  <dimension ref="A1:F72"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="B72" sqref="B72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3899,7 +3853,7 @@
       <c r="A6" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="12" t="s">
         <v>77</v>
       </c>
       <c r="C6" s="3" t="s">
@@ -3930,111 +3884,121 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="B9" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="B9" s="12" t="s">
         <v>77</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>19</v>
+        <v>82</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>20</v>
+        <v>46</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>21</v>
+        <v>172</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>23</v>
-      </c>
+      <c r="A10" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>81</v>
+        <v>173</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>77</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>78</v>
+        <v>19</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>79</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>102</v>
+        <v>175</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B12" s="3"/>
+      <c r="B12" s="12" t="s">
+        <v>77</v>
+      </c>
       <c r="C12" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="D15" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E12" s="3" t="s">
+      <c r="E15" s="3" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="4" t="s">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="3"/>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-    </row>
-    <row r="15" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>26</v>
-      </c>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="3"/>
@@ -4045,7 +4009,7 @@
     </row>
     <row r="18" spans="1:5" ht="19" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>162</v>
+        <v>87</v>
       </c>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
@@ -4054,7 +4018,7 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
-        <v>163</v>
+        <v>27</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>81</v>
@@ -4063,48 +4027,48 @@
         <v>19</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>165</v>
+        <v>29</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>166</v>
+        <v>26</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20" s="3" t="s">
-        <v>164</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>167</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A21" s="3"/>
+      <c r="A20" s="3"/>
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+    </row>
+    <row r="21" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="A21" s="5" t="s">
+        <v>162</v>
+      </c>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
       <c r="E21" s="3"/>
     </row>
-    <row r="22" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A22" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="B22" s="3"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>166</v>
+      </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
-        <v>28</v>
+        <v>164</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>81</v>
@@ -4113,153 +4077,135 @@
         <v>19</v>
       </c>
       <c r="D23" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" s="3"/>
+      <c r="B24" s="3"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+    </row>
+    <row r="25" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="A25" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="B25" s="3"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D26" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="E23" s="3" t="s">
+      <c r="E26" s="3" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A24" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="E24" s="3" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A25" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="E25" s="3" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A26" s="4" t="s">
-        <v>157</v>
-      </c>
-      <c r="B26" s="3"/>
-      <c r="C26" s="3"/>
-      <c r="D26" s="3"/>
-      <c r="E26" s="3"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
-        <v>28</v>
+        <v>158</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>81</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>82</v>
+        <v>19</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A28" s="4" t="s">
+      <c r="A28" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29" s="4" t="s">
         <v>157</v>
       </c>
-      <c r="B28" s="3"/>
-      <c r="C28" s="3"/>
-      <c r="D28" s="3"/>
-      <c r="E28" s="3"/>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A29" s="3"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>
       <c r="E29" s="3"/>
     </row>
-    <row r="30" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A30" s="5" t="s">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A30" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="B31" s="3"/>
+      <c r="C31" s="3"/>
+      <c r="D31" s="3"/>
+      <c r="E31" s="3"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32" s="3"/>
+      <c r="B32" s="3"/>
+      <c r="C32" s="3"/>
+      <c r="D32" s="3"/>
+      <c r="E32" s="3"/>
+    </row>
+    <row r="33" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="A33" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="B30" s="3"/>
-      <c r="C30" s="3"/>
-      <c r="D30" s="3"/>
-      <c r="E30" s="3"/>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A31" s="3" t="s">
+      <c r="B33" s="3"/>
+      <c r="C33" s="3"/>
+      <c r="D33" s="3"/>
+      <c r="E33" s="3"/>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A34" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="B31" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D31" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="E31" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A32" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="C32" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D32" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E32" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A33" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="C33" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D33" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="E33" s="3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A34" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="B34" s="2" t="s">
+      <c r="B34" s="12" t="s">
         <v>77</v>
       </c>
       <c r="C34" s="3" t="s">
@@ -4269,504 +4215,507 @@
         <v>34</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="B35" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B35" s="12" t="s">
         <v>77</v>
       </c>
       <c r="C35" s="3" t="s">
         <v>19</v>
       </c>
       <c r="D35" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A36" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B36" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D36" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="E35" s="3" t="s">
+      <c r="E36" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A37" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B37" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E37" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A38" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B38" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E38" s="3" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A36" s="3" t="s">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A39" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B36" s="3" t="s">
+      <c r="B39" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="C36" s="3" t="s">
+      <c r="C39" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="D36" s="3" t="s">
+      <c r="D39" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="E36" s="3" t="s">
+      <c r="E39" s="3" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A37" s="4" t="s">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A40" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="B37" s="3"/>
-      <c r="C37" s="3"/>
-      <c r="D37" s="3"/>
-      <c r="E37" s="3"/>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A38" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="B38" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="C38" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="D38" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E38" s="3" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A39" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="B39" s="3"/>
-      <c r="C39" s="3"/>
-      <c r="D39" s="3"/>
-      <c r="E39" s="3"/>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A40" s="3"/>
       <c r="B40" s="3"/>
       <c r="C40" s="3"/>
       <c r="D40" s="3"/>
       <c r="E40" s="3"/>
     </row>
-    <row r="41" spans="1:6" ht="19" x14ac:dyDescent="0.25">
-      <c r="A41" s="5" t="s">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A41" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E41" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A42" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="B42" s="3"/>
+      <c r="C42" s="3"/>
+      <c r="D42" s="3"/>
+      <c r="E42" s="3"/>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A43" s="3"/>
+      <c r="B43" s="3"/>
+      <c r="C43" s="3"/>
+      <c r="D43" s="3"/>
+      <c r="E43" s="3"/>
+    </row>
+    <row r="44" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="A44" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="B41" s="3"/>
-      <c r="C41" s="3"/>
-      <c r="D41" s="3"/>
-      <c r="E41" s="3"/>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A42" s="3" t="s">
+      <c r="B44" s="3"/>
+      <c r="C44" s="3"/>
+      <c r="D44" s="3"/>
+      <c r="E44" s="3"/>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A45" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="B42" s="2" t="s">
+      <c r="B45" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="C42" s="3" t="s">
+      <c r="C45" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D42" s="3" t="s">
+      <c r="D45" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="E42" s="3" t="s">
+      <c r="E45" s="3" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A43" s="3" t="s">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A46" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="B43" s="2" t="s">
+      <c r="B46" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="C43" s="3" t="s">
+      <c r="C46" s="3" t="s">
         <v>19</v>
-      </c>
-      <c r="D43" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="E43" s="3" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A44" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="C44" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="D44" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="E44" s="3" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A45" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="B45" s="3"/>
-      <c r="C45" s="3"/>
-      <c r="D45" s="3"/>
-      <c r="E45" s="3"/>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A46" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="B46" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="C46" s="3" t="s">
-        <v>82</v>
       </c>
       <c r="D46" s="3" t="s">
         <v>68</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A47" s="4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A47" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="D47" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="E47" s="3" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A48" s="4" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A48" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="B48" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="C48" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="D48" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="E48" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="F48" s="3"/>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B48" s="3"/>
+      <c r="C48" s="3"/>
+      <c r="D48" s="3"/>
+      <c r="E48" s="3"/>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" s="3" t="s">
-        <v>71</v>
+        <v>98</v>
       </c>
       <c r="B49" s="3" t="s">
         <v>81</v>
       </c>
       <c r="C49" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="D49" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="E49" s="3" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A50" s="4" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A51" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="D51" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="E51" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="F51" s="3"/>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A52" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C52" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="D49" s="3" t="s">
+      <c r="D52" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="E49" s="3" t="s">
+      <c r="E52" s="3" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A50" s="3"/>
-      <c r="B50" s="3"/>
-      <c r="C50" s="3"/>
-      <c r="D50" s="3"/>
-      <c r="E50" s="3"/>
-    </row>
-    <row r="51" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A51" s="5" t="s">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A53" s="3"/>
+      <c r="B53" s="3"/>
+      <c r="C53" s="3"/>
+      <c r="D53" s="3"/>
+      <c r="E53" s="3"/>
+    </row>
+    <row r="54" spans="1:6" ht="19" x14ac:dyDescent="0.25">
+      <c r="A54" s="5" t="s">
         <v>133</v>
       </c>
-      <c r="B51" s="3"/>
-      <c r="C51" s="3"/>
-      <c r="D51" s="3"/>
-      <c r="E51" s="3"/>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A52" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="B52" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="C52" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D52" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="E52" s="3" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A53" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="B53" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="C53" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D53" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="E53" s="3" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A54" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="B54" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="C54" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D54" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="E54" s="3" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B54" s="3"/>
+      <c r="C54" s="3"/>
+      <c r="D54" s="3"/>
+      <c r="E54" s="3"/>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="B55" s="3" t="s">
+      <c r="B55" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="C55" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D55" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="E55" s="3" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A56" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="B56" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="C56" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D56" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="E56" s="3" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A57" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="B57" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="C57" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D57" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="E57" s="3" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A58" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="B58" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="C55" s="3" t="s">
+      <c r="C58" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="D55" s="3" t="s">
+      <c r="D58" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="E55" s="3" t="s">
+      <c r="E58" s="3" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A56" s="4" t="s">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A59" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="B56" s="3"/>
-      <c r="C56" s="3"/>
-      <c r="D56" s="3"/>
-      <c r="E56" s="3"/>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A57" s="3" t="s">
+      <c r="B59" s="3"/>
+      <c r="C59" s="3"/>
+      <c r="D59" s="3"/>
+      <c r="E59" s="3"/>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A60" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="B57" s="3" t="s">
+      <c r="B60" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="C57" s="3" t="s">
+      <c r="C60" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="D57" s="3" t="s">
+      <c r="D60" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="E57" s="3" t="s">
+      <c r="E60" s="3" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A58" s="4" t="s">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A61" s="4" t="s">
         <v>131</v>
-      </c>
-      <c r="B58" s="3"/>
-      <c r="C58" s="3"/>
-      <c r="D58" s="3"/>
-      <c r="E58" s="3"/>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A59" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="B59" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="C59" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="D59" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="E59" s="3" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A60" s="3"/>
-      <c r="B60" s="3"/>
-      <c r="C60" s="3"/>
-      <c r="D60" s="3"/>
-      <c r="E60" s="3"/>
-    </row>
-    <row r="61" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A61" s="5" t="s">
-        <v>93</v>
       </c>
       <c r="B61" s="3"/>
       <c r="C61" s="3"/>
       <c r="D61" s="3"/>
       <c r="E61" s="3"/>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="B62" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C62" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="D62" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="E62" s="3" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A63" s="3"/>
+      <c r="B63" s="3"/>
+      <c r="C63" s="3"/>
+      <c r="D63" s="3"/>
+      <c r="E63" s="3"/>
+    </row>
+    <row r="64" spans="1:6" ht="19" x14ac:dyDescent="0.25">
+      <c r="A64" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="B64" s="3"/>
+      <c r="C64" s="3"/>
+      <c r="D64" s="3"/>
+      <c r="E64" s="3"/>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A65" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="B62" s="3" t="s">
+      <c r="B65" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="C62" s="3" t="s">
+      <c r="C65" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D62" s="3" t="s">
+      <c r="D65" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="E62" s="3" t="s">
+      <c r="E65" s="3" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A63" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="B63" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="C63" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D63" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="E63" s="3" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A64" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="B64" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="C64" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="D64" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="E64" s="3" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A65" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="B65" s="3"/>
-      <c r="C65" s="3"/>
-      <c r="D65" s="3"/>
-      <c r="E65" s="3"/>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="B66" s="3" t="s">
-        <v>81</v>
+        <v>73</v>
+      </c>
+      <c r="B66" s="12" t="s">
+        <v>77</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>82</v>
+        <v>19</v>
       </c>
       <c r="D66" s="3" t="s">
         <v>74</v>
       </c>
       <c r="E66" s="3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A68" s="5" t="s">
-        <v>111</v>
-      </c>
+        <v>75</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A67" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B67" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C67" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="D67" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="E67" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A68" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="B68" s="3"/>
+      <c r="C68" s="3"/>
+      <c r="D68" s="3"/>
+      <c r="E68" s="3"/>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69" s="3" t="s">
-        <v>44</v>
+        <v>96</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="C69" s="3" t="s">
         <v>82</v>
       </c>
       <c r="D69" s="3" t="s">
-        <v>46</v>
+        <v>74</v>
       </c>
       <c r="E69" s="3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A70" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="B70" s="3"/>
-      <c r="C70" s="3"/>
-      <c r="D70" s="3"/>
-      <c r="E70" s="3"/>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A71" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="B71" s="3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="A71" s="5" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A72" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="B72" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="C71" s="3" t="s">
+      <c r="C72" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D71" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="E71" s="3" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A73" s="5" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A74" s="3" t="s">
-        <v>148</v>
-      </c>
-      <c r="B74" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="C74" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D74" s="3" t="s">
+      <c r="D72" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="E74" s="3" t="s">
+      <c r="E72" s="3" t="s">
         <v>147</v>
       </c>
     </row>
@@ -4777,6 +4726,249 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D7FB9C0-6D9B-EA43-86CE-62488FCDBEBD}">
+  <dimension ref="A2:E25"/>
+  <sheetViews>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13:XFD13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="16.33203125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="18" style="3" customWidth="1"/>
+    <col min="3" max="16384" width="10.83203125" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="4"/>
+    </row>
+    <row r="4" spans="1:5" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+    </row>
+    <row r="5" spans="1:5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+    </row>
+    <row r="7" spans="1:5" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+    </row>
+    <row r="8" spans="1:5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A9" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+    </row>
+    <row r="10" spans="1:5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A11" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A12" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A13" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A14" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A15" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A16" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A465CD1-D6F7-9041-8A2D-50A1485B8A1E}">
   <dimension ref="A2:F5"/>
   <sheetViews>
@@ -4827,7 +5019,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2B163E5-67A7-084D-A911-402169A79C95}">
   <dimension ref="A2:F6"/>
   <sheetViews>
@@ -4896,7 +5088,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC0F426C-1745-574D-951C-4E7769C56B92}">
   <dimension ref="A2:F10"/>
   <sheetViews>
@@ -5021,7 +5213,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E8BAF33-DE4E-1E4F-AD2E-75B314F497B5}">
   <dimension ref="A2:F7"/>
   <sheetViews>
@@ -5100,7 +5292,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACCCEC27-64BC-994D-B48B-D371CCD95FCF}">
   <dimension ref="A2:F12"/>
   <sheetViews>
@@ -5244,113 +5436,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88D14B79-96F7-D04D-9879-B8E70751AAF2}">
-  <dimension ref="A2:E9"/>
-  <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="31.33203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
-        <v>135</v>
-      </c>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>